<commit_message>
Add/edit and delete complete for job preference
</commit_message>
<xml_diff>
--- a/DailyTaskSheet.xlsx
+++ b/DailyTaskSheet.xlsx
@@ -42,23 +42,7 @@
 3)Planned for required Api to be required for project</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">naman-tatvasoft/JobApplicationPortal (github.com)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">naman-tatvasoft/JobApplicationPortal (github.com) </t>
   </si>
   <si>
     <t xml:space="preserve">8hr 45min</t>
@@ -107,7 +91,8 @@
   <si>
     <t xml:space="preserve">1)Custom exception added to all modules
 2)Email sent to employer when candidate applies
-3)Testing of all Api's till now completed</t>
+3)Testing of all Api's till now completed
+4)Minor bug fixing</t>
   </si>
   <si>
     <t xml:space="preserve">8hr 31min</t>
@@ -132,6 +117,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -152,12 +138,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,32 +190,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,140 +346,160 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="65.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>45814</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>45817</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="75.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>45818</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
         <v>45819</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
         <v>45820</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
         <v>45821</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
         <v>45824</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>6</v>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>45825</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>45826</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>45827</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>45828</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
-    <hyperlink ref="D3" r:id="rId2" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
-    <hyperlink ref="D4" r:id="rId3" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
-    <hyperlink ref="D5" r:id="rId4" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
-    <hyperlink ref="D6" r:id="rId5" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
-    <hyperlink ref="D7" r:id="rId6" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
-    <hyperlink ref="D8" r:id="rId7" display="naman-tatvasoft/JobApplicationPortal (github.com)"/>
+    <hyperlink ref="D2" r:id="rId1" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D3" r:id="rId2" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D4" r:id="rId3" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D5" r:id="rId4" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D6" r:id="rId5" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D7" r:id="rId6" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D8" r:id="rId7" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Helper for email sending
</commit_message>
<xml_diff>
--- a/DailyTaskSheet.xlsx
+++ b/DailyTaskSheet.xlsx
@@ -106,7 +106,8 @@
   <si>
     <t xml:space="preserve">1)Create,Update and Delete job preference by candidate
 2)Mail sent after job creation to candidate with matching job preference
-3)Testing</t>
+3)Helper function for email sent
+4)Testing</t>
   </si>
 </sst>
 </file>
@@ -117,7 +118,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -152,12 +153,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -201,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,10 +227,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -363,7 +354,7 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -493,7 +484,7 @@
       <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resume/cover letter upload restricted to pdf only
</commit_message>
<xml_diff>
--- a/DailyTaskSheet.xlsx
+++ b/DailyTaskSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -118,7 +118,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -152,6 +152,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,6 +233,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -354,8 +364,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,9 +487,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>45825</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>19</v>
@@ -491,6 +504,9 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>45826</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,6 +529,7 @@
     <hyperlink ref="D7" r:id="rId6" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
     <hyperlink ref="D8" r:id="rId7" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
     <hyperlink ref="D9" r:id="rId8" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D10" r:id="rId9" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Converted validations from data annotations to fluent validator
</commit_message>
<xml_diff>
--- a/DailyTaskSheet.xlsx
+++ b/DailyTaskSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -116,6 +116,9 @@
     <t xml:space="preserve">1)Restrict file upload type to pdf
 2)Added Rate limiting for API’s
 3)Improved In-memory filtering and sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Changed data annotation to fluent validations</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,6 +163,17 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +249,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -363,7 +385,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -517,6 +539,12 @@
       <c r="A11" s="4" t="n">
         <v>45827</v>
       </c>
+      <c r="C11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -534,6 +562,7 @@
     <hyperlink ref="D8" r:id="rId7" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
     <hyperlink ref="D9" r:id="rId8" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
     <hyperlink ref="D10" r:id="rId9" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
+    <hyperlink ref="D11" r:id="rId10" display="naman-tatvasoft/JobApplicationPortal (github.com) "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>